<commit_message>
4 logic of notes and multiple code issues
</commit_message>
<xml_diff>
--- a/LOGS/39b47cb4-af4d-4cc7-ac2a-0c79a3780657/main_page_service_output/main_pages.xlsx
+++ b/LOGS/39b47cb4-af4d-4cc7-ac2a-0c79a3780657/main_page_service_output/main_pages.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="101">
   <si>
     <t>Particulars</t>
   </si>
@@ -187,130 +187,130 @@
     <t>26</t>
   </si>
   <si>
+    <t>assets</t>
+  </si>
+  <si>
+    <t>equity_liabilities</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>noncurrent</t>
+  </si>
+  <si>
+    <t>equity</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Cost of sales</t>
+  </si>
+  <si>
+    <t>Employee benefits expense</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Finance costs</t>
+  </si>
+  <si>
+    <t>Occupancy</t>
+  </si>
+  <si>
+    <t>Other expenses</t>
+  </si>
+  <si>
+    <t>Loss before income tax benefit</t>
+  </si>
+  <si>
+    <t>Income tax benefit</t>
+  </si>
+  <si>
+    <t>Loss after income tax benefit for the year attributable to the owners of Precise Air Group (Holdings) Pty Limited and Controlled Entities</t>
+  </si>
+  <si>
+    <t>Other comprehensive income for the year, net of tax</t>
+  </si>
+  <si>
+    <t>Total comprehensive loss for the year attributable to the owners of Precise Air</t>
+  </si>
+  <si>
+    <t>Group (Holdings) Pty Limited and Controlled Entities</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Cash flows from operating activities</t>
+  </si>
+  <si>
+    <t>Receipts from customers</t>
+  </si>
+  <si>
+    <t>Payments to suppliers and employees</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>Interest and other finance costs paid</t>
+  </si>
+  <si>
+    <t>Income taxes refunded</t>
+  </si>
+  <si>
+    <t>Net cash from operating activities</t>
+  </si>
+  <si>
+    <t>Cash flows from investing activities</t>
+  </si>
+  <si>
+    <t>Payments for property, plant and equipment</t>
+  </si>
+  <si>
+    <t>Proceeds from disposal of property, plant and equipment</t>
+  </si>
+  <si>
+    <t>Net cash used in investing activities</t>
+  </si>
+  <si>
+    <t>Cash flows from financing activities</t>
+  </si>
+  <si>
+    <t>Proceeds from issue of shares</t>
+  </si>
+  <si>
+    <t>Repayment of hire purchase lease liabilities</t>
+  </si>
+  <si>
+    <t>Repayment of borrowings</t>
+  </si>
+  <si>
+    <t>Repayment of lease liabilities</t>
+  </si>
+  <si>
+    <t>Net cash from/(used in) financing activities</t>
+  </si>
+  <si>
+    <t>Net increase/decrease) in cash and cash equivalents</t>
+  </si>
+  <si>
+    <t>Cash and cash equivalents at the beginning of the financial year</t>
+  </si>
+  <si>
+    <t>Cash and cash equivalents at the end of the financial year</t>
+  </si>
+  <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>assets</t>
-  </si>
-  <si>
-    <t>equity_liabilities</t>
-  </si>
-  <si>
-    <t>current</t>
-  </si>
-  <si>
-    <t>noncurrent</t>
-  </si>
-  <si>
-    <t>equity</t>
-  </si>
-  <si>
-    <t>Revenue</t>
-  </si>
-  <si>
-    <t>Expenses</t>
-  </si>
-  <si>
-    <t>Cost of sales</t>
-  </si>
-  <si>
-    <t>Employee benefits expense</t>
-  </si>
-  <si>
-    <t>Depreciation</t>
-  </si>
-  <si>
-    <t>Finance costs</t>
-  </si>
-  <si>
-    <t>Occupancy</t>
-  </si>
-  <si>
-    <t>Other expenses</t>
-  </si>
-  <si>
-    <t>Loss before income tax benefit</t>
-  </si>
-  <si>
-    <t>Income tax benefit</t>
-  </si>
-  <si>
-    <t>Loss after income tax benefit for the year attributable to the owners of Precise Air Group (Holdings) Pty Limited and Controlled Entities</t>
-  </si>
-  <si>
-    <t>Other comprehensive income for the year, net of tax</t>
-  </si>
-  <si>
-    <t>Total comprehensive loss for the year attributable to the owners of Precise Air</t>
-  </si>
-  <si>
-    <t>Group (Holdings) Pty Limited and Controlled Entities</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Cash flows from operating activities</t>
-  </si>
-  <si>
-    <t>Receipts from customers</t>
-  </si>
-  <si>
-    <t>Payments to suppliers and employees</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>Interest and other finance costs paid</t>
-  </si>
-  <si>
-    <t>Income taxes refunded</t>
-  </si>
-  <si>
-    <t>Net cash from operating activities</t>
-  </si>
-  <si>
-    <t>Cash flows from investing activities</t>
-  </si>
-  <si>
-    <t>Payments for property, plant and equipment</t>
-  </si>
-  <si>
-    <t>Proceeds from disposal of property, plant and equipment</t>
-  </si>
-  <si>
-    <t>Net cash used in investing activities</t>
-  </si>
-  <si>
-    <t>Cash flows from financing activities</t>
-  </si>
-  <si>
-    <t>Proceeds from issue of shares</t>
-  </si>
-  <si>
-    <t>Repayment of hire purchase lease liabilities</t>
-  </si>
-  <si>
-    <t>Repayment of borrowings</t>
-  </si>
-  <si>
-    <t>Repayment of lease liabilities</t>
-  </si>
-  <si>
-    <t>Net cash from/(used in) financing activities</t>
-  </si>
-  <si>
-    <t>Net increase/decrease) in cash and cash equivalents</t>
-  </si>
-  <si>
-    <t>Cash and cash equivalents at the beginning of the financial year</t>
-  </si>
-  <si>
-    <t>Cash and cash equivalents at the end of the financial year</t>
   </si>
   <si>
     <t>operating_activities</t>
@@ -677,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -714,10 +714,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -731,10 +731,10 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -751,10 +751,10 @@
         <v>1543537</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -771,10 +771,10 @@
         <v>21734371</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -791,10 +791,10 @@
         <v>239846</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -811,10 +811,10 @@
         <v>3332245</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -831,10 +831,10 @@
         <v>365183</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -851,10 +851,10 @@
         <v>1122015</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -868,10 +868,10 @@
         <v>28337197</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -885,10 +885,10 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -905,10 +905,10 @@
         <v>6284865</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -925,10 +925,10 @@
         <v>2368526</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -945,10 +945,10 @@
         <v>1627273</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -965,10 +965,10 @@
         <v>1832902</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -982,10 +982,10 @@
         <v>12113566</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1002,7 +1002,7 @@
         <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1016,10 +1016,10 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" t="s">
         <v>58</v>
-      </c>
-      <c r="F18" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1033,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
         <v>58</v>
-      </c>
-      <c r="F19" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1053,10 +1053,10 @@
         <v>13141957</v>
       </c>
       <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
         <v>58</v>
-      </c>
-      <c r="F20" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1073,10 +1073,10 @@
         <v>1300741</v>
       </c>
       <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
         <v>58</v>
-      </c>
-      <c r="F21" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1093,10 +1093,10 @@
         <v>1929062</v>
       </c>
       <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" t="s">
         <v>58</v>
-      </c>
-      <c r="F22" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1113,10 +1113,10 @@
         <v>4274326</v>
       </c>
       <c r="E23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" t="s">
         <v>58</v>
-      </c>
-      <c r="F23" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1133,10 +1133,10 @@
         <v>1784939</v>
       </c>
       <c r="E24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" t="s">
         <v>58</v>
-      </c>
-      <c r="F24" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1150,10 +1150,10 @@
         <v>22431025</v>
       </c>
       <c r="E25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" t="s">
         <v>58</v>
-      </c>
-      <c r="F25" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1167,10 +1167,10 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1187,10 +1187,10 @@
         <v>4500000</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1207,10 +1207,10 @@
         <v>2968818</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1227,10 +1227,10 @@
         <v>389670</v>
       </c>
       <c r="E29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1244,10 +1244,10 @@
         <v>7858488</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1261,7 +1261,7 @@
         <v>30289513</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
         <v>60</v>
@@ -1278,7 +1278,7 @@
         <v>10161250</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
         <v>60</v>
@@ -1295,10 +1295,10 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1315,10 +1315,10 @@
         <v>5014754</v>
       </c>
       <c r="E34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1335,10 +1335,10 @@
         <v>5146496</v>
       </c>
       <c r="E35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1352,710 +1352,10 @@
         <v>10161250</v>
       </c>
       <c r="E36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F36" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37" t="s">
-        <v>58</v>
-      </c>
-      <c r="F37" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="B38" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38">
-        <v>2023</v>
-      </c>
-      <c r="D38">
-        <v>2022</v>
-      </c>
-      <c r="E38" t="s">
-        <v>58</v>
-      </c>
-      <c r="F38" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>58</v>
-      </c>
-      <c r="F39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41" t="s">
-        <v>57</v>
-      </c>
-      <c r="F41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42">
-        <v>3813586</v>
-      </c>
-      <c r="D42">
-        <v>1543537</v>
-      </c>
-      <c r="E42" t="s">
-        <v>57</v>
-      </c>
-      <c r="F42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43">
-        <v>19697457</v>
-      </c>
-      <c r="D43">
-        <v>21734371</v>
-      </c>
-      <c r="E43" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>239846</v>
-      </c>
-      <c r="E44" t="s">
-        <v>57</v>
-      </c>
-      <c r="F44" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" t="s">
-        <v>39</v>
-      </c>
-      <c r="C45">
-        <v>3707538</v>
-      </c>
-      <c r="D45">
-        <v>3332245</v>
-      </c>
-      <c r="E45" t="s">
-        <v>57</v>
-      </c>
-      <c r="F45" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>365183</v>
-      </c>
-      <c r="E46" t="s">
-        <v>57</v>
-      </c>
-      <c r="F46" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47">
-        <v>2077138</v>
-      </c>
-      <c r="D47">
-        <v>1122015</v>
-      </c>
-      <c r="E47" t="s">
-        <v>57</v>
-      </c>
-      <c r="F47" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48">
-        <v>29295719</v>
-      </c>
-      <c r="D48">
-        <v>28337197</v>
-      </c>
-      <c r="E48" t="s">
-        <v>57</v>
-      </c>
-      <c r="F48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49" t="s">
-        <v>57</v>
-      </c>
-      <c r="F49" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50">
-        <v>5629485</v>
-      </c>
-      <c r="D50">
-        <v>6284865</v>
-      </c>
-      <c r="E50" t="s">
-        <v>57</v>
-      </c>
-      <c r="F50" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51" t="s">
-        <v>43</v>
-      </c>
-      <c r="C51">
-        <v>4407236</v>
-      </c>
-      <c r="D51">
-        <v>2368526</v>
-      </c>
-      <c r="E51" t="s">
-        <v>57</v>
-      </c>
-      <c r="F51" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52">
-        <v>1627273</v>
-      </c>
-      <c r="D52">
-        <v>1627273</v>
-      </c>
-      <c r="E52" t="s">
-        <v>57</v>
-      </c>
-      <c r="F52" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>17</v>
-      </c>
-      <c r="B53" t="s">
-        <v>45</v>
-      </c>
-      <c r="C53">
-        <v>2313929</v>
-      </c>
-      <c r="D53">
-        <v>1832902</v>
-      </c>
-      <c r="E53" t="s">
-        <v>57</v>
-      </c>
-      <c r="F53" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>18</v>
-      </c>
-      <c r="C54">
-        <v>13977923</v>
-      </c>
-      <c r="D54">
-        <v>12113566</v>
-      </c>
-      <c r="E54" t="s">
-        <v>57</v>
-      </c>
-      <c r="F54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C55">
-        <v>43273642</v>
-      </c>
-      <c r="D55">
-        <v>40450763</v>
-      </c>
-      <c r="E55" t="s">
-        <v>57</v>
-      </c>
-      <c r="F55" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56" t="s">
-        <v>58</v>
-      </c>
-      <c r="F56" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>21</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57" t="s">
-        <v>58</v>
-      </c>
-      <c r="F57" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" t="s">
-        <v>22</v>
-      </c>
-      <c r="B58" t="s">
-        <v>46</v>
-      </c>
-      <c r="C58">
-        <v>14583624</v>
-      </c>
-      <c r="D58">
-        <v>13141957</v>
-      </c>
-      <c r="E58" t="s">
-        <v>58</v>
-      </c>
-      <c r="F58" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" t="s">
-        <v>23</v>
-      </c>
-      <c r="B59" t="s">
-        <v>47</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-      <c r="D59">
-        <v>1300741</v>
-      </c>
-      <c r="E59" t="s">
-        <v>58</v>
-      </c>
-      <c r="F59" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>24</v>
-      </c>
-      <c r="B60" t="s">
-        <v>48</v>
-      </c>
-      <c r="C60">
-        <v>1603877</v>
-      </c>
-      <c r="D60">
-        <v>1929062</v>
-      </c>
-      <c r="E60" t="s">
-        <v>58</v>
-      </c>
-      <c r="F60" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" t="s">
-        <v>49</v>
-      </c>
-      <c r="C61">
-        <v>4005793</v>
-      </c>
-      <c r="D61">
-        <v>4274326</v>
-      </c>
-      <c r="E61" t="s">
-        <v>58</v>
-      </c>
-      <c r="F61" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" t="s">
-        <v>50</v>
-      </c>
-      <c r="C62">
-        <v>1315030</v>
-      </c>
-      <c r="D62">
-        <v>1784939</v>
-      </c>
-      <c r="E62" t="s">
-        <v>58</v>
-      </c>
-      <c r="F62" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="s">
-        <v>27</v>
-      </c>
-      <c r="C63">
-        <v>21508324</v>
-      </c>
-      <c r="D63">
-        <v>22431025</v>
-      </c>
-      <c r="E63" t="s">
-        <v>58</v>
-      </c>
-      <c r="F63" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
-        <v>28</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64" t="s">
-        <v>58</v>
-      </c>
-      <c r="F64" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
-        <v>23</v>
-      </c>
-      <c r="B65" t="s">
-        <v>51</v>
-      </c>
-      <c r="C65">
-        <v>3500000</v>
-      </c>
-      <c r="D65">
-        <v>4500000</v>
-      </c>
-      <c r="E65" t="s">
-        <v>58</v>
-      </c>
-      <c r="F65" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B66" t="s">
-        <v>52</v>
-      </c>
-      <c r="C66">
-        <v>4013764</v>
-      </c>
-      <c r="D66">
-        <v>2968818</v>
-      </c>
-      <c r="E66" t="s">
-        <v>58</v>
-      </c>
-      <c r="F66" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" t="s">
-        <v>25</v>
-      </c>
-      <c r="B67" t="s">
-        <v>53</v>
-      </c>
-      <c r="C67">
-        <v>293491</v>
-      </c>
-      <c r="D67">
-        <v>389670</v>
-      </c>
-      <c r="E67" t="s">
-        <v>58</v>
-      </c>
-      <c r="F67" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" t="s">
-        <v>29</v>
-      </c>
-      <c r="C68">
-        <v>7807255</v>
-      </c>
-      <c r="D68">
-        <v>7858488</v>
-      </c>
-      <c r="E68" t="s">
-        <v>58</v>
-      </c>
-      <c r="F68" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" t="s">
-        <v>30</v>
-      </c>
-      <c r="C69">
-        <v>29315579</v>
-      </c>
-      <c r="D69">
-        <v>30289513</v>
-      </c>
-      <c r="E69" t="s">
-        <v>58</v>
-      </c>
-      <c r="F69" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
-        <v>31</v>
-      </c>
-      <c r="C70">
-        <v>13958063</v>
-      </c>
-      <c r="D70">
-        <v>10161250</v>
-      </c>
-      <c r="E70" t="s">
-        <v>58</v>
-      </c>
-      <c r="F70" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" t="s">
-        <v>32</v>
-      </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71" t="s">
-        <v>58</v>
-      </c>
-      <c r="F71" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" t="s">
-        <v>33</v>
-      </c>
-      <c r="B72" t="s">
-        <v>54</v>
-      </c>
-      <c r="C72">
-        <v>10014754</v>
-      </c>
-      <c r="D72">
-        <v>5014754</v>
-      </c>
-      <c r="E72" t="s">
-        <v>58</v>
-      </c>
-      <c r="F72" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" t="s">
-        <v>34</v>
-      </c>
-      <c r="B73" t="s">
-        <v>55</v>
-      </c>
-      <c r="C73">
-        <v>3943309</v>
-      </c>
-      <c r="D73">
-        <v>5146496</v>
-      </c>
-      <c r="E73" t="s">
-        <v>58</v>
-      </c>
-      <c r="F73" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" t="s">
-        <v>35</v>
-      </c>
-      <c r="C74">
-        <v>13958063</v>
-      </c>
-      <c r="D74">
-        <v>10161250</v>
-      </c>
-      <c r="E74" t="s">
-        <v>58</v>
-      </c>
-      <c r="F74" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2099,10 +1399,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2">
         <v>121891318</v>
@@ -2113,7 +1413,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2124,7 +1424,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>-90975382</v>
@@ -2135,7 +1435,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5">
         <v>-19123030</v>
@@ -2146,7 +1446,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6">
         <v>-2131132</v>
@@ -2157,7 +1457,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>-401327</v>
@@ -2168,7 +1468,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8">
         <v>-305833</v>
@@ -2179,7 +1479,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9">
         <v>-10638828</v>
@@ -2190,7 +1490,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10">
         <v>-1684214</v>
@@ -2201,10 +1501,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11">
         <v>481027</v>
@@ -2215,7 +1515,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
         <v>55</v>
@@ -2229,7 +1529,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2240,7 +1540,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2251,7 +1551,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15">
         <v>-1203187</v>
@@ -2295,7 +1595,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2309,7 +1609,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3">
         <v>132061551</v>
@@ -2323,7 +1623,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4">
         <v>-129685372</v>
@@ -2337,7 +1637,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5">
         <v>2376179</v>
@@ -2351,7 +1651,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6">
         <v>-401327</v>
@@ -2365,7 +1665,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7">
         <v>239846</v>
@@ -2379,7 +1679,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8">
         <v>2214698</v>
@@ -2393,7 +1693,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2407,7 +1707,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -2424,7 +1724,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11">
         <v>354416</v>
@@ -2438,7 +1738,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12">
         <v>-601407</v>
@@ -2452,7 +1752,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2466,7 +1766,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s">
         <v>54</v>
@@ -2483,7 +1783,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15">
         <v>-1307263</v>
@@ -2497,7 +1797,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16">
         <v>-1000000</v>
@@ -2511,7 +1811,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17">
         <v>-735238</v>
@@ -2525,7 +1825,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18">
         <v>1957499</v>
@@ -2539,7 +1839,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19">
         <v>3570790</v>
@@ -2553,7 +1853,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20">
         <v>242796</v>
@@ -2567,7 +1867,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
@@ -2584,7 +1884,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2598,10 +1898,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2615,7 +1915,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2629,7 +1929,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25">
         <v>132061551</v>
@@ -2643,7 +1943,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26">
         <v>-129685372</v>
@@ -2657,7 +1957,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27">
         <v>2376179</v>
@@ -2671,7 +1971,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28">
         <v>-401327</v>
@@ -2685,7 +1985,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29">
         <v>239846</v>
@@ -2699,7 +1999,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30">
         <v>2214698</v>
@@ -2713,7 +2013,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2727,7 +2027,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
         <v>42</v>
@@ -2744,7 +2044,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33">
         <v>354416</v>
@@ -2758,7 +2058,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34">
         <v>-601407</v>
@@ -2772,7 +2072,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2786,7 +2086,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
         <v>54</v>
@@ -2803,7 +2103,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37">
         <v>-1307263</v>
@@ -2817,7 +2117,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38">
         <v>-1000000</v>
@@ -2831,7 +2131,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39">
         <v>-735238</v>
@@ -2845,7 +2145,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40">
         <v>1957499</v>
@@ -2859,7 +2159,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41">
         <v>3570790</v>
@@ -2873,7 +2173,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42">
         <v>242796</v>
@@ -2887,7 +2187,7 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B43" t="s">
         <v>36</v>

</xml_diff>